<commit_message>
reading table from excel file
</commit_message>
<xml_diff>
--- a/src/test/resources/testing_excel.xlsx
+++ b/src/test/resources/testing_excel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{548FD9B4-E816-445C-AC60-B6643ACC8F84}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7173C16-53C8-44AB-B156-08D5564C8A63}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -365,7 +365,7 @@
   <dimension ref="J7:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -400,9 +400,7 @@
       <c r="J9" s="1">
         <v>1541616</v>
       </c>
-      <c r="K9" s="1">
-        <v>4564</v>
-      </c>
+      <c r="K9" s="1"/>
       <c r="L9" s="1" t="s">
         <v>4</v>
       </c>

</xml_diff>